<commit_message>
Agregamos análisis finales y seed al script de simulación.
</commit_message>
<xml_diff>
--- a/punto_3.xlsx
+++ b/punto_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lator\Documents\workspace\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{20B5C3CC-64AF-4CBB-85E8-9364E71BF0C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1827F84-E5EC-4469-9C28-C0D2C369C562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
   <si>
     <t>pivot</t>
   </si>
@@ -43,7 +43,7 @@
     <t>0.61980642139303</t>
   </si>
   <si>
-    <t>0.9534</t>
+    <t>0.955</t>
   </si>
   <si>
     <t>pivot_2</t>
@@ -52,7 +52,7 @@
     <t>0.614470737764349</t>
   </si>
   <si>
-    <t>0.9528</t>
+    <t>0.9498</t>
   </si>
   <si>
     <t>pivot_3</t>
@@ -61,49 +61,37 @@
     <t>0.357845404236729</t>
   </si>
   <si>
-    <t>0.952</t>
+    <t>0.9484</t>
   </si>
   <si>
     <t>0.356799390286126</t>
   </si>
   <si>
-    <t>0.949</t>
+    <t>0.945</t>
   </si>
   <si>
     <t>0.196000000000019</t>
   </si>
   <si>
-    <t>0.9522</t>
+    <t>0.9468</t>
   </si>
   <si>
     <t>0.195824782511175</t>
   </si>
   <si>
+    <t>0.9472</t>
+  </si>
+  <si>
     <t>0.0619806421393033</t>
   </si>
   <si>
-    <t>0.956</t>
+    <t>0.9474</t>
   </si>
   <si>
     <t>0.0619740664085953</t>
   </si>
   <si>
-    <t>0.9558</t>
-  </si>
-  <si>
-    <t>0.9556</t>
-  </si>
-  <si>
-    <t>0.9454</t>
-  </si>
-  <si>
-    <t>0.955</t>
-  </si>
-  <si>
-    <t>0.9524</t>
-  </si>
-  <si>
-    <t>0.95</t>
+    <t>0.9464</t>
   </si>
 </sst>
 </file>
@@ -961,16 +949,14 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection sqref="A1:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,7 +1109,7 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,7 +1126,7 @@
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1154,10 +1140,10 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1171,10 +1157,10 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E12" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1188,10 +1174,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1194,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1225,7 +1211,7 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,7 +1228,7 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,7 +1245,7 @@
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,7 +1262,7 @@
         <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,7 +1279,7 @@
         <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1310,7 +1296,7 @@
         <v>16</v>
       </c>
       <c r="E20" t="s">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,7 +1313,7 @@
         <v>18</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,7 +1330,7 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1358,10 +1344,10 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1375,10 +1361,10 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1392,10 +1378,10 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Arreglamos el pivote 2 y corremos los script otra vez.
</commit_message>
<xml_diff>
--- a/punto_3.xlsx
+++ b/punto_3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lator\Documents\workspace\tp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1827F84-E5EC-4469-9C28-C0D2C369C562}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E666D500-5AC0-40CD-81B8-614960730720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="33">
   <si>
     <t>pivot</t>
   </si>
@@ -49,21 +49,33 @@
     <t>pivot_2</t>
   </si>
   <si>
+    <t>0.149779999999995</t>
+  </si>
+  <si>
+    <t>0.9494</t>
+  </si>
+  <si>
+    <t>pivot_3</t>
+  </si>
+  <si>
     <t>0.614470737764349</t>
   </si>
   <si>
     <t>0.9498</t>
   </si>
   <si>
-    <t>pivot_3</t>
-  </si>
-  <si>
     <t>0.357845404236729</t>
   </si>
   <si>
     <t>0.9484</t>
   </si>
   <si>
+    <t>0.0499266666666646</t>
+  </si>
+  <si>
+    <t>0.9468</t>
+  </si>
+  <si>
     <t>0.356799390286126</t>
   </si>
   <si>
@@ -73,7 +85,10 @@
     <t>0.196000000000019</t>
   </si>
   <si>
-    <t>0.9468</t>
+    <t>0.0149779999999994</t>
+  </si>
+  <si>
+    <t>0.9508</t>
   </si>
   <si>
     <t>0.195824782511175</t>
@@ -88,10 +103,22 @@
     <t>0.9474</t>
   </si>
   <si>
+    <t>0.0014978000000001</t>
+  </si>
+  <si>
+    <t>0.9476</t>
+  </si>
+  <si>
     <t>0.0619740664085953</t>
   </si>
   <si>
     <t>0.9464</t>
+  </si>
+  <si>
+    <t>0.149779999999994</t>
+  </si>
+  <si>
+    <t>0.0499266666666647</t>
   </si>
 </sst>
 </file>
@@ -949,14 +976,15 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E25"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -1021,10 +1049,10 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,10 +1066,10 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1055,10 +1083,10 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,10 +1100,10 @@
         <v>2</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1089,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E8" t="s">
         <v>17</v>
@@ -1106,10 +1134,10 @@
         <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1123,10 +1151,10 @@
         <v>2</v>
       </c>
       <c r="D10" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1140,10 +1168,10 @@
         <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1157,10 +1185,10 @@
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,10 +1202,10 @@
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1208,7 +1236,7 @@
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
@@ -1225,10 +1253,10 @@
         <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1242,10 +1270,10 @@
         <v>5</v>
       </c>
       <c r="D17" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1259,10 +1287,10 @@
         <v>5</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1276,10 +1304,10 @@
         <v>5</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1293,7 +1321,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E20" t="s">
         <v>17</v>
@@ -1310,10 +1338,10 @@
         <v>5</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1327,10 +1355,10 @@
         <v>5</v>
       </c>
       <c r="D22" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1344,10 +1372,10 @@
         <v>5</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1361,10 +1389,10 @@
         <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E24" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1378,16 +1406,17 @@
         <v>5</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>